<commit_message>
v1.2 Made assumptions on the Question answers
due to no reply on the SIQ from the customers , i made assumptions to answer the questions
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH-SIQ.xlsx
+++ b/LH_REQUIREMENTS/LH-SIQ.xlsx
@@ -8,19 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CA30A3-FF23-4DDF-9469-7A6684EE1781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39ACD12E-3622-4B84-918C-08D77052F4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
+    <sheet name="SIQ" sheetId="1" r:id="rId1"/>
+    <sheet name="Version history" sheetId="4" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="Table2">#REF!</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
   <si>
     <t>ID</t>
   </si>
@@ -158,13 +162,64 @@
   </si>
   <si>
     <t xml:space="preserve"> Should the admin features include removing articles, videos, and audio files?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>a text showing all the password requirements to the user</t>
+  </si>
+  <si>
+    <t>no comment</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>4 categories</t>
+  </si>
+  <si>
+    <t>100MB</t>
+  </si>
+  <si>
+    <t>Version number</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Created SIQ sheet</t>
+  </si>
+  <si>
+    <t>Mahmoud Radi</t>
+  </si>
+  <si>
+    <t>Updated the SIQ sheet according to the review comments</t>
+  </si>
+  <si>
+    <t>Made assumptions on the Question answers</t>
+  </si>
+  <si>
+    <t>Updated section</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -188,6 +243,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -203,7 +265,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -346,26 +408,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -385,9 +432,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -400,9 +444,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -410,9 +451,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -425,11 +463,23 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,6 +537,18 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Question"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Answer"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Comments"/>
+  </tableColumns>
+  <tableStyleInfo name="Sheet3-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9563CCC3-851B-453C-933D-17087BDF14C3}" name="Table16" displayName="Table16" ref="A1:D19">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C89EB1EC-4C2E-4603-9648-9FD01BCB32E7}" name="Version number"/>
+    <tableColumn id="2" xr3:uid="{A294B132-8A15-431C-AEB5-4D6FD0930374}" name="Author"/>
+    <tableColumn id="4" xr3:uid="{3E3C5CEB-EBA5-4F13-AEF1-F4BAEA5407AE}" name="Updated section"/>
+    <tableColumn id="5" xr3:uid="{108D32EB-91AA-4ED5-8D1C-98D9C6F8BE4E}" name="Date"/>
   </tableColumns>
   <tableStyleInfo name="Sheet3-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -695,9 +757,9 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+    <sheetView zoomScale="59" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -706,7 +768,7 @@
     <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="99.88671875" customWidth="1"/>
     <col min="4" max="4" width="48" customWidth="1"/>
-    <col min="5" max="5" width="64.109375" customWidth="1"/>
+    <col min="5" max="5" width="71.44140625" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -728,7 +790,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -737,24 +799,32 @@
       <c r="C2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
+      <c r="D2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
+      <c r="D3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -763,25 +833,33 @@
       <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="8"/>
-      <c r="I4" s="15"/>
+      <c r="D4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="13"/>
+      <c r="D5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -790,167 +868,219 @@
       <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="8"/>
+      <c r="D6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="13"/>
+      <c r="D7" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="8"/>
+      <c r="D8" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="13"/>
+      <c r="D9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="8"/>
+      <c r="D10" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="13"/>
+      <c r="D11" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="8"/>
+      <c r="D12" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="13"/>
+      <c r="D13" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="8"/>
+      <c r="D14" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="13"/>
+      <c r="D15" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="8"/>
+      <c r="D16" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="13"/>
+      <c r="D17" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22"/>
+      <c r="D18" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
+      <c r="A19" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -966,4 +1096,181 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34FB6AEB-FB0F-423F-B9F5-E6539C732705}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="99.88671875" customWidth="1"/>
+    <col min="4" max="4" width="48" customWidth="1"/>
+    <col min="5" max="5" width="64.109375" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="22">
+        <v>45752</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="22">
+        <v>45754</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="22">
+        <v>45759</v>
+      </c>
+      <c r="H4" s="13"/>
+    </row>
+    <row r="5" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" showDropDown="1" sqref="B19" xr:uid="{1EA06F4F-72F6-4F21-A23E-D13EF2576099}"/>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Yes or NO" sqref="C19" xr:uid="{CA5276C0-DEDC-4E02-A3A0-20173513E8E1}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
v1.3 Added questions about the login module and answers assumptions
added the missing questions about the login module and assumed the answers according to the understanding of how the login module should work
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH-SIQ.xlsx
+++ b/LH_REQUIREMENTS/LH-SIQ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39ACD12E-3622-4B84-918C-08D77052F4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAACD6B7-BFF9-4B33-B046-D1C40C08C92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SIQ" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -213,6 +213,36 @@
   </si>
   <si>
     <t>1.2</t>
+  </si>
+  <si>
+    <t>Added questions about the login module and answers assumptions</t>
+  </si>
+  <si>
+    <t>LH-SIQ-018</t>
+  </si>
+  <si>
+    <t>LH-SIQ-019</t>
+  </si>
+  <si>
+    <t>LH-SIQ-020</t>
+  </si>
+  <si>
+    <t>LH-SIQ-021</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Should the user login using the username and password?</t>
+  </si>
+  <si>
+    <t>Should only registered users be able to login?</t>
+  </si>
+  <si>
+    <t>Should we store registrants passwords using Hashing and SALT?</t>
+  </si>
+  <si>
+    <t>Should there be a generic error message if the user enters wrong email or password or leaves any of them empty</t>
   </si>
 </sst>
 </file>
@@ -530,7 +560,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E22">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Feature"/>
@@ -755,11 +785,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView zoomScale="59" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="59" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1080,15 +1110,80 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Yes or NO" sqref="D2:D19" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Yes or NO" sqref="D2:D22" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showDropDown="1" sqref="B2:C19" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="B2:C22" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1102,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34FB6AEB-FB0F-423F-B9F5-E6539C732705}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScale="68" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1174,10 +1269,18 @@
       <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="A5" s="8">
+        <v>1.3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="22">
+        <v>45760</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>

</xml_diff>

<commit_message>
v1.3 Add some questions after creation SRS
ask some more questions about login , registration and ID constrain after creation SRS
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH-SIQ.xlsx
+++ b/LH_REQUIREMENTS/LH-SIQ.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\pulled repo\Group-3-Learning-hub\LH_REQUIREMENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAACD6B7-BFF9-4B33-B046-D1C40C08C92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SIQ" sheetId="1" r:id="rId1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="82">
   <si>
     <t>ID</t>
   </si>
@@ -215,9 +214,6 @@
     <t>1.2</t>
   </si>
   <si>
-    <t>Added questions about the login module and answers assumptions</t>
-  </si>
-  <si>
     <t>LH-SIQ-018</t>
   </si>
   <si>
@@ -227,29 +223,60 @@
     <t>LH-SIQ-020</t>
   </si>
   <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Should users log in exclusively using their email and password</t>
+  </si>
+  <si>
+    <t>Should the system allow only registered users to login</t>
+  </si>
+  <si>
+    <t>Should all login errors (invalid password, empty fields, unregistered email) show 
+the same generic message (e.g., 'Invalid credentials</t>
+  </si>
+  <si>
+    <t>Should passwords be stored securely using hashing and salting</t>
+  </si>
+  <si>
     <t>LH-SIQ-021</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Should the user login using the username and password?</t>
-  </si>
-  <si>
-    <t>Should only registered users be able to login?</t>
-  </si>
-  <si>
-    <t>Should we store registrants passwords using Hashing and SALT?</t>
-  </si>
-  <si>
-    <t>Should there be a generic error message if the user enters wrong email or password or leaves any of them empty</t>
+    <t>Should all fields (email, username, password) be mandatory in the registration form</t>
+  </si>
+  <si>
+    <t>Should the username have specific constraints (e.g., 4-20 characters, no special symbols)</t>
+  </si>
+  <si>
+    <t>Should successful registration create exactly one user account (no duplicates)</t>
+  </si>
+  <si>
+    <t>Should the system auto-generate user IDs in a specific format</t>
+  </si>
+  <si>
+    <t>LH-SIQ-022</t>
+  </si>
+  <si>
+    <t>LH-SIQ-023</t>
+  </si>
+  <si>
+    <t>LH-SIQ-024</t>
+  </si>
+  <si>
+    <t>LH-SIQ-025</t>
+  </si>
+  <si>
+    <t>Ahmed Abuzaid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add some questions about login , registration and ID constrain after creation SRS </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -260,12 +287,8 @@
       <sz val="15"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Roboto"/>
     </font>
     <font>
       <sz val="8"/>
@@ -279,6 +302,20 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="3">
@@ -295,7 +332,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -350,36 +387,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF284E3F"/>
       </left>
       <right style="thin">
@@ -395,46 +402,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF6F8F9"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FFF6F8F9"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FFF6F8F9"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFF6F8F9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF6F8F9"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF6F8F9"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFF6F8F9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -442,80 +419,88 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="0"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -542,10 +527,10 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle name="Sheet3-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="secondRowStripe" dxfId="0"/>
+    <tableStyle name="Sheet3-style" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="4"/>
+      <tableStyleElement type="firstRowStripe" dxfId="3"/>
+      <tableStyleElement type="secondRowStripe" dxfId="2"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -560,25 +545,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E26" headerRowDxfId="1">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Feature"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Question"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Answer"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Comments"/>
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="Feature"/>
+    <tableColumn id="3" name="Question"/>
+    <tableColumn id="4" name="Answer"/>
+    <tableColumn id="5" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="Sheet3-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9563CCC3-851B-453C-933D-17087BDF14C3}" name="Table16" displayName="Table16" ref="A1:D19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="A1:D19" headerRowDxfId="0">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C89EB1EC-4C2E-4603-9648-9FD01BCB32E7}" name="Version number"/>
-    <tableColumn id="2" xr3:uid="{A294B132-8A15-431C-AEB5-4D6FD0930374}" name="Author"/>
-    <tableColumn id="4" xr3:uid="{3E3C5CEB-EBA5-4F13-AEF1-F4BAEA5407AE}" name="Updated section"/>
-    <tableColumn id="5" xr3:uid="{108D32EB-91AA-4ED5-8D1C-98D9C6F8BE4E}" name="Date"/>
+    <tableColumn id="1" name="Version number"/>
+    <tableColumn id="2" name="Author"/>
+    <tableColumn id="4" name="Updated section"/>
+    <tableColumn id="5" name="Date"/>
   </tableColumns>
   <tableStyleInfo name="Sheet3-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -781,409 +766,445 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+    <sheetView zoomScale="59" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="40.15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="99.88671875" customWidth="1"/>
+    <col min="3" max="3" width="99.85546875" customWidth="1"/>
     <col min="4" max="4" width="48" customWidth="1"/>
-    <col min="5" max="5" width="71.44140625" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="79.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="15" customFormat="1" ht="40.15" customHeight="1">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:9" ht="40.15" customHeight="1">
+      <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:9" ht="40.15" customHeight="1">
+      <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:9" ht="40.15" customHeight="1">
+      <c r="A4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="I4" s="13"/>
-    </row>
-    <row r="5" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="40.15" customHeight="1">
+      <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:9" ht="40.15" customHeight="1">
+      <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:9" ht="40.15" customHeight="1">
+      <c r="A7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:9" ht="40.15" customHeight="1">
+      <c r="A8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:9" ht="40.15" customHeight="1">
+      <c r="A9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:9" ht="40.15" customHeight="1">
+      <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:9" ht="40.15" customHeight="1">
+      <c r="A11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:9" ht="40.15" customHeight="1">
+      <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:9" ht="40.15" customHeight="1">
+      <c r="A13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:9" ht="40.15" customHeight="1">
+      <c r="A14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:9" ht="40.15" customHeight="1">
+      <c r="A15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:9" ht="40.15" customHeight="1">
+      <c r="A16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:5" ht="40.15" customHeight="1">
+      <c r="A17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="18" spans="1:5" ht="40.15" customHeight="1">
+      <c r="A18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="19" spans="1:5" ht="40.15" customHeight="1">
+      <c r="A19" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="1:5" ht="40.15" customHeight="1">
+      <c r="A20" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B20" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" spans="1:5" ht="56.25">
+      <c r="A21" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="17" t="s">
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="1:5" ht="40.15" customHeight="1">
+      <c r="A22" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="17" t="s">
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="1:5" ht="40.15" customHeight="1">
+      <c r="A23" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="16" t="s">
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+    </row>
+    <row r="24" spans="1:5" ht="40.15" customHeight="1">
+      <c r="A24" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>48</v>
-      </c>
+      <c r="C24" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="1:5" ht="40.15" customHeight="1">
+      <c r="A25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="1:5" ht="40.15" customHeight="1">
+      <c r="A26" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Yes or NO" sqref="D2:D22" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Yes or NO" sqref="D2:D26">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showDropDown="1" sqref="B2:C22" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="C2:C18 B2:B26"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1194,180 +1215,180 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34FB6AEB-FB0F-423F-B9F5-E6539C732705}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScale="68" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="99.88671875" customWidth="1"/>
+    <col min="3" max="3" width="99.85546875" customWidth="1"/>
     <col min="4" max="4" width="48" customWidth="1"/>
-    <col min="5" max="5" width="64.109375" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="64.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:8" s="15" customFormat="1" ht="40.15" customHeight="1">
+      <c r="A1" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:8" ht="40.15" customHeight="1">
+      <c r="A2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="4">
         <v>45752</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:8" ht="40.15" customHeight="1">
+      <c r="A3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="4">
         <v>45754</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:8" ht="40.15" customHeight="1">
+      <c r="A4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="4">
         <v>45759</v>
       </c>
-      <c r="H4" s="13"/>
-    </row>
-    <row r="5" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="40.15" customHeight="1">
+      <c r="A5" s="1">
         <v>1.3</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="22">
+      <c r="B5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="4">
         <v>45760</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+    <row r="6" spans="1:8" ht="40.15" customHeight="1">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="40.15" customHeight="1">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="40.15" customHeight="1">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="40.15" customHeight="1">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="40.15" customHeight="1">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="40.15" customHeight="1">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="40.15" customHeight="1">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="40.15" customHeight="1">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="40.15" customHeight="1">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="40.15" customHeight="1">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="40.15" customHeight="1">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" ht="40.15" customHeight="1">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" ht="40.15" customHeight="1">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" ht="40.15" customHeight="1">
+      <c r="A19" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="B19" xr:uid="{1EA06F4F-72F6-4F21-A23E-D13EF2576099}"/>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Yes or NO" sqref="C19" xr:uid="{CA5276C0-DEDC-4E02-A3A0-20173513E8E1}">
+    <dataValidation allowBlank="1" showDropDown="1" sqref="B19"/>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Yes or NO" sqref="C19">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v1.4  modify SIQ template
modify SIQ template and ask some more questions about registration and ID constrain after creation SRS
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH-SIQ.xlsx
+++ b/LH_REQUIREMENTS/LH-SIQ.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\pulled repo\Group-3-Learning-hub\LH_REQUIREMENTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed Abuzaid\Downloads\qa_workshop_temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SIQ" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="83">
   <si>
     <t>ID</t>
   </si>
@@ -214,6 +214,9 @@
     <t>1.2</t>
   </si>
   <si>
+    <t>Added questions about the login module and answers assumptions</t>
+  </si>
+  <si>
     <t>LH-SIQ-018</t>
   </si>
   <si>
@@ -223,60 +226,59 @@
     <t>LH-SIQ-020</t>
   </si>
   <si>
+    <t>LH-SIQ-021</t>
+  </si>
+  <si>
     <t>Login</t>
   </si>
   <si>
-    <t>Should users log in exclusively using their email and password</t>
-  </si>
-  <si>
-    <t>Should the system allow only registered users to login</t>
-  </si>
-  <si>
-    <t>Should all login errors (invalid password, empty fields, unregistered email) show 
-the same generic message (e.g., 'Invalid credentials</t>
-  </si>
-  <si>
-    <t>Should passwords be stored securely using hashing and salting</t>
-  </si>
-  <si>
-    <t>LH-SIQ-021</t>
+    <t>Should the user login using the username and password?</t>
+  </si>
+  <si>
+    <t>Should only registered users be able to login?</t>
+  </si>
+  <si>
+    <t>Should we store registrants passwords using Hashing and SALT?</t>
+  </si>
+  <si>
+    <t>Should there be a generic error message if the user enters wrong email or password or leaves any of them empty</t>
+  </si>
+  <si>
+    <t>LH-SIQ-022</t>
   </si>
   <si>
     <t>Should all fields (email, username, password) be mandatory in the registration form</t>
   </si>
   <si>
+    <t>LH-SIQ-023</t>
+  </si>
+  <si>
     <t>Should the username have specific constraints (e.g., 4-20 characters, no special symbols)</t>
   </si>
   <si>
+    <t>LH-SIQ-024</t>
+  </si>
+  <si>
     <t>Should successful registration create exactly one user account (no duplicates)</t>
   </si>
   <si>
+    <t>LH-SIQ-025</t>
+  </si>
+  <si>
     <t>Should the system auto-generate user IDs in a specific format</t>
   </si>
   <si>
-    <t>LH-SIQ-022</t>
-  </si>
-  <si>
-    <t>LH-SIQ-023</t>
-  </si>
-  <si>
-    <t>LH-SIQ-024</t>
-  </si>
-  <si>
-    <t>LH-SIQ-025</t>
-  </si>
-  <si>
     <t>Ahmed Abuzaid</t>
   </si>
   <si>
-    <t xml:space="preserve">Add some questions about login , registration and ID constrain after creation SRS </t>
+    <t xml:space="preserve">Add some questions registration and ID constrain after creation SRS and modify SIQ template </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -297,11 +299,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="15"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="0"/>
+      <name val="Roboto"/>
     </font>
     <font>
       <b/>
@@ -309,7 +317,6 @@
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -317,8 +324,14 @@
       <color theme="0"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,12 +340,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF356854"/>
-        <bgColor rgb="FF356854"/>
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F8F9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -342,164 +367,393 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF284E3F"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF356854"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF284E3F"/>
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF284E3F"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF356854"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF356854"/>
+        <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color rgb="FF284E3F"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color rgb="FF284E3F"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF356854"/>
+        <color indexed="64"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color rgb="FF284E3F"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF284E3F"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF284E3F"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF284E3F"/>
+        <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color rgb="FFF6F8F9"/>
-      </right>
+      <right/>
       <top style="thin">
-        <color rgb="FFF6F8F9"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFF6F8F9"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="15" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="12">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="16"/>
+        <sz val="15"/>
         <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="0"/>
-      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -528,9 +782,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Sheet3-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="4"/>
-      <tableStyleElement type="firstRowStripe" dxfId="3"/>
-      <tableStyleElement type="secondRowStripe" dxfId="2"/>
+      <tableStyleElement type="headerRow" dxfId="11"/>
+      <tableStyleElement type="firstRowStripe" dxfId="10"/>
+      <tableStyleElement type="secondRowStripe" dxfId="9"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -545,20 +799,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E26" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E26" headerRowDxfId="8" totalsRowDxfId="5" headerRowBorderDxfId="7" tableBorderDxfId="6">
   <tableColumns count="5">
-    <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="Feature"/>
-    <tableColumn id="3" name="Question"/>
-    <tableColumn id="4" name="Answer"/>
-    <tableColumn id="5" name="Comments"/>
+    <tableColumn id="1" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" name="Feature" dataDxfId="3"/>
+    <tableColumn id="3" name="Question" dataDxfId="2"/>
+    <tableColumn id="4" name="Answer" dataDxfId="1"/>
+    <tableColumn id="5" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Sheet3-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="A1:D19" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="A1:D18">
   <tableColumns count="4">
     <tableColumn id="1" name="Version number"/>
     <tableColumn id="2" name="Author"/>
@@ -774,7 +1028,7 @@
   <sheetViews>
     <sheetView zoomScale="59" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="40.15" customHeight="1"/>
@@ -787,20 +1041,20 @@
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="15" customFormat="1" ht="40.15" customHeight="1">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:9" ht="40.15" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -817,7 +1071,7 @@
       <c r="D2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -834,7 +1088,7 @@
       <c r="D3" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -851,10 +1105,10 @@
       <c r="D4" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="40.15" customHeight="1">
       <c r="A5" s="6" t="s">
@@ -869,7 +1123,7 @@
       <c r="D5" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -886,7 +1140,7 @@
       <c r="D6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -903,7 +1157,7 @@
       <c r="D7" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -911,7 +1165,7 @@
       <c r="A8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -920,7 +1174,7 @@
       <c r="D8" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -928,7 +1182,7 @@
       <c r="A9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -937,7 +1191,7 @@
       <c r="D9" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="10" t="s">
         <v>50</v>
       </c>
     </row>
@@ -945,7 +1199,7 @@
       <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -954,7 +1208,7 @@
       <c r="D10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="10" t="s">
         <v>51</v>
       </c>
     </row>
@@ -962,7 +1216,7 @@
       <c r="A11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -971,7 +1225,7 @@
       <c r="D11" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -979,7 +1233,7 @@
       <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -988,7 +1242,7 @@
       <c r="D12" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -996,7 +1250,7 @@
       <c r="A13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -1005,7 +1259,7 @@
       <c r="D13" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1013,7 +1267,7 @@
       <c r="A14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -1022,7 +1276,7 @@
       <c r="D14" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1030,7 +1284,7 @@
       <c r="A15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -1039,7 +1293,7 @@
       <c r="D15" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1047,7 +1301,7 @@
       <c r="A16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -1056,7 +1310,7 @@
       <c r="D16" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1064,7 +1318,7 @@
       <c r="A17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -1073,7 +1327,7 @@
       <c r="D17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1081,7 +1335,7 @@
       <c r="A18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -1090,113 +1344,129 @@
       <c r="D18" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="10" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="40.15" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>68</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
+        <v>69</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="40.15" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="40.15" customHeight="1">
+      <c r="A21" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="B21" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="1:5" ht="56.25">
-      <c r="A21" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>66</v>
-      </c>
       <c r="C21" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
+        <v>72</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="40.15" customHeight="1">
       <c r="A22" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
+      <c r="D22" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="40.15" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>35</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
+        <v>74</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="13"/>
     </row>
     <row r="24" spans="1:5" ht="40.15" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>35</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
+        <v>76</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5" ht="40.15" customHeight="1">
       <c r="A25" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="1:5" ht="40.15" customHeight="1">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
+      <c r="C26" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1204,7 +1474,7 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Yes or NO" sqref="D2:D26">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showDropDown="1" sqref="C2:C18 B2:B26"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="B2:C26"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1219,7 +1489,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
@@ -1227,19 +1497,19 @@
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="99.85546875" customWidth="1"/>
-    <col min="4" max="4" width="48" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="64.140625" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="15" customFormat="1" ht="40.15" customHeight="1">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:8" ht="40.15" customHeight="1">
+      <c r="A1" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="20" t="s">
         <v>59</v>
       </c>
       <c r="D1" s="19" t="s">
@@ -1247,148 +1517,159 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="40.15" customHeight="1">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="23">
         <v>45752</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="40.15" customHeight="1">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="26">
         <v>45754</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="40.15" customHeight="1">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="26">
         <v>45759</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="40.15" customHeight="1">
-      <c r="A5" s="1">
+      <c r="A5" s="21">
         <v>1.3</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="26">
+        <v>45760</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="40.15" customHeight="1">
+      <c r="A6" s="29">
+        <v>1.4</v>
+      </c>
+      <c r="B6" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="4">
+      <c r="C6" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="31">
         <v>45760</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="40.15" customHeight="1">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
     <row r="7" spans="1:8" ht="40.15" customHeight="1">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:8" ht="40.15" customHeight="1">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
     </row>
     <row r="9" spans="1:8" ht="40.15" customHeight="1">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
     </row>
     <row r="10" spans="1:8" ht="40.15" customHeight="1">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
     </row>
     <row r="11" spans="1:8" ht="40.15" customHeight="1">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
     </row>
     <row r="12" spans="1:8" ht="40.15" customHeight="1">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
     </row>
     <row r="13" spans="1:8" ht="40.15" customHeight="1">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
     </row>
     <row r="14" spans="1:8" ht="40.15" customHeight="1">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
     </row>
     <row r="15" spans="1:8" ht="40.15" customHeight="1">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
     </row>
     <row r="16" spans="1:8" ht="40.15" customHeight="1">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
     </row>
     <row r="17" spans="1:4" ht="40.15" customHeight="1">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
     </row>
     <row r="18" spans="1:4" ht="40.15" customHeight="1">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" ht="40.15" customHeight="1">
-      <c r="A19" s="1"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="B19"/>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Yes or NO" sqref="C19">
+    <dataValidation allowBlank="1" showDropDown="1" sqref="B18"/>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Yes or NO" sqref="C18">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v1.5 modify SIQ after review
modify SIQ after get the comments from last version of siq review "v1.2" on login, registration an ID constrains
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH-SIQ.xlsx
+++ b/LH_REQUIREMENTS/LH-SIQ.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed Abuzaid\Downloads\qa_workshop_temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\pulled repo\Group-3-Learning-hub\LH_REQUIREMENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="SIQ" sheetId="1" r:id="rId1"/>
@@ -70,9 +70,6 @@
     <t>ADMIN Constrain</t>
   </si>
   <si>
-    <t>Should the admin Features include deleting a user?</t>
-  </si>
-  <si>
     <t>Should the Max number of users on the Website be 50 users?</t>
   </si>
   <si>
@@ -235,43 +232,46 @@
     <t>Should the user login using the username and password?</t>
   </si>
   <si>
-    <t>Should only registered users be able to login?</t>
-  </si>
-  <si>
-    <t>Should we store registrants passwords using Hashing and SALT?</t>
-  </si>
-  <si>
-    <t>Should there be a generic error message if the user enters wrong email or password or leaves any of them empty</t>
-  </si>
-  <si>
     <t>LH-SIQ-022</t>
   </si>
   <si>
-    <t>Should all fields (email, username, password) be mandatory in the registration form</t>
-  </si>
-  <si>
     <t>LH-SIQ-023</t>
   </si>
   <si>
-    <t>Should the username have specific constraints (e.g., 4-20 characters, no special symbols)</t>
-  </si>
-  <si>
     <t>LH-SIQ-024</t>
   </si>
   <si>
-    <t>Should successful registration create exactly one user account (no duplicates)</t>
-  </si>
-  <si>
     <t>LH-SIQ-025</t>
   </si>
   <si>
-    <t>Should the system auto-generate user IDs in a specific format</t>
-  </si>
-  <si>
     <t>Ahmed Abuzaid</t>
   </si>
   <si>
     <t xml:space="preserve">Add some questions registration and ID constrain after creation SRS and modify SIQ template </t>
+  </si>
+  <si>
+    <t>Should the admin be able to remove a user from the system?</t>
+  </si>
+  <si>
+    <t>Should access to the system be restricted to users who have registered?</t>
+  </si>
+  <si>
+    <t>Should the system display a simple error message if login information is incorrect or incomplete?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should user passwords be stored securely using basic hashing methods? </t>
+  </si>
+  <si>
+    <t>Should the registration form require all fields (email, username, and password) to be filled out?</t>
+  </si>
+  <si>
+    <t>Should the username have specific constraints (e.g., 4-20 characters,only contain letters and numbers  no special symbols like(!,@,#,$&lt;%,^,etc))</t>
+  </si>
+  <si>
+    <t>Should the system prevent multiple registrations using the same email or username?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Should the system automatically assign user IDs in a simple, consistent format (e.g., U001, U002)?</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1026,7 @@
   </sheetPr>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView zoomScale="59" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="59" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
@@ -1060,110 +1060,110 @@
     </row>
     <row r="2" spans="1:9" ht="40.15" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="40.15" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="40.15" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>47</v>
       </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="40.15" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="40.15" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="40.15" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="40.15" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>8</v>
@@ -1172,134 +1172,134 @@
         <v>9</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="40.15" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="40.15" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="40.15" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="40.15" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="40.15" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="40.15" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="40.15" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="40.15" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>12</v>
@@ -1308,162 +1308,162 @@
         <v>13</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="40.15" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="40.15" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="40.15" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>69</v>
-      </c>
       <c r="D19" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="40.15" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="40.15" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="40.15" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="40.15" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="13"/>
     </row>
     <row r="24" spans="1:5" ht="40.15" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5" ht="40.15" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="13"/>
     </row>
     <row r="26" spans="1:5" ht="40.15" customHeight="1">
       <c r="A26" s="14" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="18"/>
@@ -1488,7 +1488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
+    <sheetView zoomScale="68" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1504,27 +1504,27 @@
   <sheetData>
     <row r="1" spans="1:8" ht="40.15" customHeight="1">
       <c r="A1" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>53</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="40.15" customHeight="1">
       <c r="A2" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="23">
         <v>45752</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="3" spans="1:8" ht="40.15" customHeight="1">
       <c r="A3" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>56</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>57</v>
       </c>
       <c r="D3" s="26">
         <v>45754</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="4" spans="1:8" ht="40.15" customHeight="1">
       <c r="A4" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="26">
         <v>45759</v>
@@ -1564,10 +1564,10 @@
         <v>1.3</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" s="26">
         <v>45760</v>
@@ -1578,10 +1578,10 @@
         <v>1.4</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D6" s="31">
         <v>45760</v>

</xml_diff>